<commit_message>
solicitud gráfica de rec210_MA_10_01_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion01/SOLICITUD_GRAFICA_REC_210.xlsx
+++ b/fuentes/contenidos/grado10/guion01/SOLICITUD_GRAFICA_REC_210.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PLANETA_2015\RECURSOS_GRECO\DECIMO\MA_10_01_CO\SOLICITUD_GRAFICA_REC_210\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado10\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5376" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5370" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="194">
   <si>
     <t>Fecha:</t>
   </si>
@@ -593,9 +593,6 @@
     <t xml:space="preserve">Imagen diseñada </t>
   </si>
   <si>
-    <t>Ilustración</t>
-  </si>
-  <si>
     <t>Las características globales de las funciones</t>
   </si>
   <si>
@@ -612,15 +609,6 @@
   </si>
   <si>
     <t>Ubicar en la pregunta 3  la imagen  de la página shutterstock cod: 359188805</t>
-  </si>
-  <si>
-    <t>Ubicar en la pregunta 4  la imagen img_01    que se encuentran en la carpeta adjunta</t>
-  </si>
-  <si>
-    <t>Ubicar en la pregunta 5  la imagen  de la página shutterstock cod: 274645046</t>
-  </si>
-  <si>
-    <t>Ubicar en la pregunta 6  la imagen  de la página shutterstock cod: 330983213</t>
   </si>
 </sst>
 </file>
@@ -1766,7 +1754,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1788,15 +1776,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1036320</xdr:colOff>
+          <xdr:colOff>1038225</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>236220</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1843,15 +1831,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1051560</xdr:colOff>
+          <xdr:colOff>1047750</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>868680</xdr:colOff>
+          <xdr:colOff>866775</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>236220</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1898,15 +1886,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>236220</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1955,13 +1943,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>480060</xdr:rowOff>
+          <xdr:rowOff>476250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1021080</xdr:colOff>
+          <xdr:colOff>1019175</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>716280</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2008,15 +1996,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1013460</xdr:colOff>
+          <xdr:colOff>1009650</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>480060</xdr:rowOff>
+          <xdr:rowOff>476250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>830580</xdr:colOff>
+          <xdr:colOff>828675</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>716280</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2063,15 +2051,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>480060</xdr:rowOff>
+          <xdr:rowOff>476250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>716280</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2118,15 +2106,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>480060</xdr:rowOff>
+          <xdr:rowOff>476250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>716280</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2496,31 +2484,31 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.19921875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.19921875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.59765625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="20.3984375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.8984375" style="15" customWidth="1"/>
-    <col min="11" max="11" width="29.59765625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="20.3984375" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="34.875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="10.8984375" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.8984375" style="2"/>
+    <col min="14" max="15" width="10.875" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2539,7 +2527,7 @@
         <v>Ubicación de la imagen en el recurso M101</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>121</v>
@@ -2570,7 +2558,7 @@
         <v>M3A</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2599,13 +2587,13 @@
         <v>M5A</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="5"/>
@@ -2631,7 +2619,7 @@
         <v>M6A</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2662,7 +2650,7 @@
         <v>M7A</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2686,13 +2674,13 @@
         <v>M8A</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -2715,7 +2703,7 @@
         <v>M9B</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2782,20 +2770,20 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
       <c r="B10" s="62">
-        <v>192215372</v>
+        <v>359188805</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso M101</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E10" s="63" t="s">
         <v>155</v>
@@ -2817,7 +2805,7 @@
         <v>500 x 500 px</v>
       </c>
       <c r="J10" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
@@ -2825,20 +2813,20 @@
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="62">
-        <v>369261434</v>
+      <c r="B11" s="62" t="s">
+        <v>187</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso M101</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E11" s="63" t="s">
         <v>155</v>
@@ -2860,7 +2848,7 @@
         <v>500 x 500 px</v>
       </c>
       <c r="J11" s="63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K11" s="65"/>
       <c r="O11" s="2" t="str">
@@ -2868,20 +2856,20 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
       <c r="B12" s="62">
-        <v>359188805</v>
+        <v>274645046</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso M101</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E12" s="63" t="s">
         <v>155</v>
@@ -2903,7 +2891,7 @@
         <v>500 x 500 px</v>
       </c>
       <c r="J12" s="63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K12" s="64"/>
       <c r="O12" s="2" t="str">
@@ -2911,136 +2899,112 @@
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>IMG04</v>
-      </c>
-      <c r="B13" s="62" t="s">
-        <v>187</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B13" s="62"/>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso M101</v>
-      </c>
-      <c r="D13" s="63" t="s">
-        <v>188</v>
-      </c>
-      <c r="E13" s="63" t="s">
-        <v>155</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
       <c r="F13" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>MA_10_01_REC210_IMG04n.png</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>286 x 286 px</v>
+        <v/>
       </c>
       <c r="H13" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_10_01_REC210_IMG04a.png</v>
+        <v/>
       </c>
       <c r="I13" s="13" t="str">
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>500 x 500 px</v>
-      </c>
-      <c r="J13" s="63" t="s">
-        <v>195</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J13" s="63"/>
       <c r="K13" s="64"/>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>IMG05</v>
-      </c>
-      <c r="B14" s="62">
-        <v>274645046</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B14" s="62"/>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso M101</v>
-      </c>
-      <c r="D14" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="E14" s="63" t="s">
-        <v>155</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
       <c r="F14" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>MA_10_01_REC210_IMG05n.png</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>286 x 286 px</v>
+        <v/>
       </c>
       <c r="H14" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_10_01_REC210_IMG05a.png</v>
+        <v/>
       </c>
       <c r="I14" s="13" t="str">
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>500 x 500 px</v>
-      </c>
-      <c r="J14" s="63" t="s">
-        <v>196</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J14" s="63"/>
       <c r="K14" s="64"/>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>IMG06</v>
-      </c>
-      <c r="B15" s="62">
-        <v>330983213</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B15" s="62"/>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso M101</v>
-      </c>
-      <c r="D15" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>155</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
       <c r="F15" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>MA_10_01_REC210_IMG06n.png</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="G15" s="13" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>286 x 286 px</v>
+        <v/>
       </c>
       <c r="H15" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_10_01_REC210_IMG06a.png</v>
+        <v/>
       </c>
       <c r="I15" s="13" t="str">
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>500 x 500 px</v>
-      </c>
-      <c r="J15" s="63" t="s">
-        <v>197</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J15" s="63"/>
       <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3145,7 +3109,7 @@
         <v>F8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v/>
@@ -6017,18 +5981,18 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.19921875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="72.25" style="22" customWidth="1"/>
     <col min="2" max="2" width="11" style="22"/>
-    <col min="3" max="3" width="13.69921875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="11.19921875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="22" customWidth="1"/>
+    <col min="4" max="4" width="11.25" style="22" customWidth="1"/>
     <col min="5" max="7" width="11" style="22"/>
     <col min="8" max="11" width="11" style="22" hidden="1" customWidth="1"/>
     <col min="12" max="16384" width="11" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="93" t="s">
         <v>38</v>
       </c>
@@ -6038,7 +6002,7 @@
       <c r="E1" s="94"/>
       <c r="F1" s="95"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
@@ -6050,7 +6014,7 @@
       <c r="E2" s="98"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>43</v>
       </c>
@@ -6074,7 +6038,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>44</v>
       </c>
@@ -6102,7 +6066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>45</v>
       </c>
@@ -6129,7 +6093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -6151,7 +6115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>11</v>
       </c>
@@ -6178,7 +6142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>53</v>
       </c>
@@ -6197,7 +6161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -6216,7 +6180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>36</v>
       </c>
@@ -6235,7 +6199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="22" t="s">
         <v>32</v>
       </c>
@@ -6246,7 +6210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I12" s="22" t="s">
         <v>37</v>
       </c>
@@ -6257,7 +6221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="93" t="s">
         <v>41</v>
       </c>
@@ -6276,7 +6240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -6293,7 +6257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>46</v>
       </c>
@@ -6311,7 +6275,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>47</v>
       </c>
@@ -6335,7 +6299,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>44</v>
       </c>
@@ -6356,7 +6320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
         <v>48</v>
       </c>
@@ -6377,7 +6341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
@@ -6396,7 +6360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>51</v>
       </c>
@@ -6418,7 +6382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21" s="22" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -6435,122 +6399,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K22" s="22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K23" s="22">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K24" s="22">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K25" s="22">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K26" s="22">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K27" s="22">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K28" s="22">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K29" s="22">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K30" s="22">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K31" s="22">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K32" s="22">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K33" s="22">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K34" s="22">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K35" s="22">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="22">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K37" s="22">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K38" s="22">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K39" s="22">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K40" s="22">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K41" s="22">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K42" s="22">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K43" s="22">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K44" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K45" s="22" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6584,13 +6548,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>480060</xdr:rowOff>
+                    <xdr:rowOff>476250</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1021080</xdr:colOff>
+                    <xdr:colOff>1019175</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>716280</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6604,15 +6568,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1013460</xdr:colOff>
+                    <xdr:colOff>1009650</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>480060</xdr:rowOff>
+                    <xdr:rowOff>476250</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>830580</xdr:colOff>
+                    <xdr:colOff>828675</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>716280</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6626,15 +6590,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>480060</xdr:rowOff>
+                    <xdr:rowOff>476250</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>716280</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6648,15 +6612,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>480060</xdr:rowOff>
+                    <xdr:rowOff>476250</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>716280</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6670,15 +6634,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1036320</xdr:colOff>
+                    <xdr:colOff>1038225</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>236220</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6692,15 +6656,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1051560</xdr:colOff>
+                    <xdr:colOff>1047750</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>868680</xdr:colOff>
+                    <xdr:colOff>866775</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>236220</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6714,15 +6678,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>236220</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6744,21 +6708,21 @@
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="22" customWidth="1"/>
-    <col min="2" max="2" width="24.19921875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="16.8984375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.69921875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.69921875" style="22" customWidth="1"/>
-    <col min="6" max="7" width="12.69921875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="24.25" style="22" customWidth="1"/>
+    <col min="3" max="3" width="16.875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.75" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.75" style="22" customWidth="1"/>
+    <col min="6" max="7" width="12.75" style="22" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="22" customWidth="1"/>
-    <col min="9" max="9" width="27.19921875" style="22" customWidth="1"/>
+    <col min="9" max="9" width="27.25" style="22" customWidth="1"/>
     <col min="10" max="10" width="44.5" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="10.69921875" style="22"/>
+    <col min="11" max="16384" width="10.75" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
         <v>56</v>
       </c>
@@ -6785,7 +6749,7 @@
       </c>
       <c r="I1" s="107"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="108"/>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
@@ -6800,7 +6764,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
@@ -6825,7 +6789,7 @@
       </c>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>57</v>
       </c>
@@ -6854,7 +6818,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>77</v>
       </c>
@@ -6883,7 +6847,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>58</v>
       </c>
@@ -6912,7 +6876,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>58</v>
       </c>
@@ -6937,7 +6901,7 @@
       </c>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>80</v>
       </c>
@@ -6966,7 +6930,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>82</v>
       </c>
@@ -6995,7 +6959,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>84</v>
       </c>
@@ -7024,7 +6988,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
         <v>86</v>
       </c>
@@ -7049,7 +7013,7 @@
       </c>
       <c r="I11" s="42"/>
     </row>
-    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
@@ -7078,7 +7042,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>91</v>
       </c>
@@ -7107,7 +7071,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>94</v>
       </c>
@@ -7130,7 +7094,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="75" t="s">
         <v>96</v>
       </c>
@@ -7156,7 +7120,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
         <v>100</v>
       </c>
@@ -7184,7 +7148,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>103</v>
       </c>
@@ -7212,7 +7176,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>184</v>
       </c>
@@ -7238,7 +7202,7 @@
       <c r="I18" s="44"/>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>137</v>
       </c>
@@ -7262,7 +7226,7 @@
       <c r="I19" s="44"/>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>137</v>
       </c>
@@ -7286,7 +7250,7 @@
       <c r="I20" s="44"/>
       <c r="J20" s="49"/>
     </row>
-    <row r="21" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>137</v>
       </c>
@@ -7310,7 +7274,7 @@
       <c r="I21" s="72"/>
       <c r="J21" s="49"/>
     </row>
-    <row r="22" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
         <v>132</v>
       </c>
@@ -7334,7 +7298,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>132</v>
       </c>
@@ -7363,7 +7327,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>134</v>
       </c>
@@ -7386,7 +7350,7 @@
       <c r="H24" s="44"/>
       <c r="I24" s="72"/>
     </row>
-    <row r="25" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
         <v>135</v>
       </c>
@@ -7410,7 +7374,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>135</v>
       </c>
@@ -7439,7 +7403,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
         <v>138</v>
       </c>
@@ -7463,7 +7427,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>138</v>
       </c>
@@ -7487,7 +7451,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
@@ -7516,7 +7480,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>139</v>
       </c>
@@ -7539,7 +7503,7 @@
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
     </row>
-    <row r="31" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
         <v>140</v>
       </c>
@@ -7556,7 +7520,7 @@
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
     </row>
-    <row r="32" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>141</v>
       </c>
@@ -7571,7 +7535,7 @@
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
         <v>136</v>
       </c>
@@ -7592,7 +7556,7 @@
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
         <v>142</v>
       </c>
@@ -7609,7 +7573,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
     </row>
-    <row r="35" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>95</v>
       </c>
@@ -7638,7 +7602,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>95</v>
       </c>
@@ -7667,7 +7631,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
         <v>143</v>
       </c>
@@ -7690,7 +7654,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
     </row>
-    <row r="38" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
         <v>143</v>
       </c>
@@ -7713,13 +7677,13 @@
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
         <v>107</v>
       </c>
       <c r="B40" s="50"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="51" t="s">
         <v>108</v>
       </c>
@@ -7733,7 +7697,7 @@
       <c r="E41" s="52"/>
       <c r="F41" s="52"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">
         <v>109</v>
       </c>
@@ -7747,7 +7711,7 @@
       <c r="E42" s="55"/>
       <c r="F42" s="55"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
         <v>110</v>
       </c>
@@ -7761,7 +7725,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="55"/>
     </row>
-    <row r="44" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="54" t="s">
         <v>111</v>
       </c>
@@ -7775,7 +7739,7 @@
       <c r="E44" s="55"/>
       <c r="F44" s="55"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
         <v>112</v>
       </c>
@@ -7789,7 +7753,7 @@
       <c r="E45" s="55"/>
       <c r="F45" s="55"/>
     </row>
-    <row r="46" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="54" t="s">
         <v>162</v>
       </c>

</xml_diff>